<commit_message>
update suppressors a bit
</commit_message>
<xml_diff>
--- a/changes/545-muzzles.xlsx
+++ b/changes/545-muzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2897338D-EEA0-4361-8F48-A37A0FDBCE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFE5564-5E36-4AD4-BC49-1BFA26B0CF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1112,7 +1112,7 @@
   <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,14 +2675,14 @@
         <v>0.32</v>
       </c>
       <c r="R23" s="2">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="S23" s="2">
         <v>-18</v>
       </c>
       <c r="T23" s="2"/>
       <c r="U23" s="2">
-        <v>-0.25</v>
+        <v>-0.2</v>
       </c>
       <c r="V23" s="2">
         <v>0.16</v>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="AA23">
         <f t="shared" ref="AA23:AA35" si="8">P23-Q23*20-R23*0.8-S23*0.6-U23*7.5+V23*15+W23/300</f>
-        <v>14.408333333333333</v>
+        <v>14.833333333333334</v>
       </c>
       <c r="AD23">
         <f t="shared" si="3"/>
@@ -2763,14 +2763,14 @@
         <v>0.3</v>
       </c>
       <c r="R24" s="2">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="S24" s="2">
         <v>-15</v>
       </c>
       <c r="T24" s="2"/>
       <c r="U24" s="2">
-        <v>-0.2</v>
+        <v>-0.15</v>
       </c>
       <c r="V24" s="2">
         <v>0.12</v>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="AA24">
         <f t="shared" si="8"/>
-        <v>14.600000000000001</v>
+        <v>15.025000000000002</v>
       </c>
       <c r="AD24">
         <f t="shared" si="3"/>
@@ -2848,14 +2848,14 @@
         <v>0.27</v>
       </c>
       <c r="R25" s="2">
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="S25" s="2">
         <v>-13</v>
       </c>
       <c r="T25" s="2"/>
       <c r="U25" s="2">
-        <v>-0.15</v>
+        <v>-0.1</v>
       </c>
       <c r="V25" s="2">
         <v>0.1</v>
@@ -2870,7 +2870,7 @@
       </c>
       <c r="AA25">
         <f t="shared" si="8"/>
-        <v>15.058333333333332</v>
+        <v>15.483333333333333</v>
       </c>
       <c r="AD25">
         <f t="shared" si="3"/>
@@ -2936,14 +2936,14 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="R26" s="2">
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="S26" s="2">
         <v>-13</v>
       </c>
       <c r="T26" s="2"/>
       <c r="U26" s="2">
-        <v>-0.15</v>
+        <v>-0.1</v>
       </c>
       <c r="V26" s="2">
         <v>0.1</v>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="AA26">
         <f t="shared" si="8"/>
-        <v>14.858333333333333</v>
+        <v>15.283333333333333</v>
       </c>
       <c r="AD26">
         <f t="shared" si="3"/>
@@ -3018,14 +3018,14 @@
         <v>0.22</v>
       </c>
       <c r="R27" s="2">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="S27" s="2">
         <v>-12</v>
       </c>
       <c r="T27" s="2"/>
       <c r="U27" s="2">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="V27" s="2">
         <v>0.06</v>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="AA27">
         <f t="shared" si="8"/>
-        <v>14.616666666666665</v>
+        <v>15.041666666666666</v>
       </c>
       <c r="AD27">
         <f t="shared" si="3"/>
@@ -3103,14 +3103,14 @@
         <v>0.23</v>
       </c>
       <c r="R28" s="2">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="S28" s="2">
         <v>-12</v>
       </c>
       <c r="T28" s="2"/>
       <c r="U28" s="2">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="V28" s="2">
         <v>0.06</v>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="AA28">
         <f t="shared" si="8"/>
-        <v>14.416666666666664</v>
+        <v>14.841666666666665</v>
       </c>
       <c r="AD28">
         <f t="shared" si="3"/>
@@ -3182,13 +3182,13 @@
         <v>0.3</v>
       </c>
       <c r="R29">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="S29">
         <v>-17</v>
       </c>
       <c r="U29">
-        <v>-0.2</v>
+        <v>-0.15</v>
       </c>
       <c r="V29">
         <v>0.14000000000000001</v>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="AA29">
         <f t="shared" si="8"/>
-        <v>14.4</v>
+        <v>14.824999999999999</v>
       </c>
       <c r="AD29">
         <f t="shared" si="3"/>

</xml_diff>